<commit_message>
TC03 TC04 Automation Scripts
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/test/resources/testData.xlsx
+++ b/InvoiceNinja/src/test/resources/testData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tasks" sheetId="9" r:id="rId9"/>
     <sheet name="Vendors" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,8 +27,19 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Iphone 12</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -155,7 +166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -332,7 +343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -342,7 +353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -368,12 +379,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>112000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
sending Projects module test cases
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/test/resources/testData.xlsx
+++ b/InvoiceNinja/src/test/resources/testData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16650" windowHeight="5415" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Tasks" sheetId="9" r:id="rId9"/>
     <sheet name="Vendors" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:S19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,8 +28,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>tyss</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>dinga</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -58,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -155,7 +171,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -332,7 +348,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -340,14 +356,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -440,12 +459,40 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>20.2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>